<commit_message>
3d graph added start of environmental effects
</commit_message>
<xml_diff>
--- a/AVG Drift for all cases.xlsx
+++ b/AVG Drift for all cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ARENA_Data\pm-analysis\pm-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DC11D1-1B79-47CE-8957-48754981990A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C4652D-D488-4CE4-A96E-E08320F3C3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{A1DEA447-5F09-4931-822D-79C9CA0DF1ED}"/>
+    <workbookView minimized="1" xWindow="760" yWindow="690" windowWidth="14400" windowHeight="8410" xr2:uid="{A1DEA447-5F09-4931-822D-79C9CA0DF1ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="44">
   <si>
     <t>Device Type</t>
   </si>
@@ -86,9 +86,6 @@
     <t>(%)</t>
   </si>
   <si>
-    <t>Kh drift per ton of CO2 absorbed</t>
-  </si>
-  <si>
     <t>pc</t>
   </si>
   <si>
@@ -158,10 +155,17 @@
     <t>curtin_uni: packed column structured packing</t>
   </si>
   <si>
-    <t>vg</t>
-  </si>
-  <si>
-    <t>counter</t>
+    <t>Kg drift per ton of CO2 absorbed</t>
+  </si>
+  <si>
+    <t>(kg/t)</t>
+  </si>
+  <si>
+    <t>Air
+ velocity</t>
+  </si>
+  <si>
+    <t>(m/s)</t>
   </si>
 </sst>
 </file>
@@ -227,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -367,20 +371,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF9CC2E5"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -433,6 +428,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -442,23 +449,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,52 +766,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD1BCC4-132E-458F-8991-6B6A5FBB7155}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A9" sqref="A9:K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -846,12 +841,15 @@
       <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="J9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="23"/>
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
@@ -876,10 +874,11 @@
       <c r="I10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="22"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="24"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -896,26 +895,25 @@
       <c r="I11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="26" t="s">
+      <c r="J11" s="21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K11" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="8">
         <v>5</v>
@@ -935,26 +933,22 @@
       <c r="J12" s="9">
         <v>0.1</v>
       </c>
-      <c r="K12" s="24">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <f>G12/(0.6*0.6)</f>
-        <v>0.91666666666666674</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K12">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="12">
         <v>5</v>
@@ -974,26 +968,22 @@
       <c r="J13" s="13">
         <v>0.1</v>
       </c>
-      <c r="K13" s="25">
-        <v>2</v>
-      </c>
-      <c r="L13">
-        <f t="shared" ref="L13:L26" si="0">G13/(0.6*0.6)</f>
-        <v>0.91666666666666674</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K13">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="C14" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="16">
         <v>3</v>
@@ -1013,26 +1003,22 @@
       <c r="J14" s="17">
         <v>0.12</v>
       </c>
-      <c r="K14" s="24">
-        <v>3</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
-        <v>0.55555555555555558</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K14">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="16">
         <v>5</v>
@@ -1052,26 +1038,22 @@
       <c r="J15" s="17">
         <v>0.16</v>
       </c>
-      <c r="K15" s="24">
-        <v>5</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
+      <c r="K15">
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="C16" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="16">
         <v>10</v>
@@ -1091,26 +1073,22 @@
       <c r="J16" s="17">
         <v>0.19</v>
       </c>
-      <c r="K16" s="24">
-        <v>7</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
-        <v>0.72222222222222232</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K16">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="12">
         <v>10</v>
@@ -1130,26 +1108,22 @@
       <c r="J17" s="13">
         <v>0.23</v>
       </c>
-      <c r="K17" s="25">
-        <v>8</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
+      <c r="K17">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="16">
         <v>15</v>
@@ -1169,26 +1143,22 @@
       <c r="J18" s="17">
         <v>0.47</v>
       </c>
-      <c r="K18" s="24">
-        <v>11</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K18">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="16">
         <v>40</v>
@@ -1208,26 +1178,22 @@
       <c r="J19" s="17">
         <v>0.59</v>
       </c>
-      <c r="K19" s="24">
-        <v>13</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>0.97222222222222221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K19">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="D20" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="12">
         <v>30</v>
@@ -1247,26 +1213,22 @@
       <c r="J20" s="13">
         <v>0.61</v>
       </c>
-      <c r="K20" s="25">
-        <v>14</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
-        <v>0.52777777777777779</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K20">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="C21" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>27</v>
-      </c>
       <c r="D21" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="16">
         <v>40</v>
@@ -1286,26 +1248,22 @@
       <c r="J21" s="17">
         <v>0.77</v>
       </c>
-      <c r="K21" s="24">
-        <v>17</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
+      <c r="K21">
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="16">
         <v>30</v>
@@ -1325,26 +1283,22 @@
       <c r="J22" s="17">
         <v>1</v>
       </c>
-      <c r="K22" s="24">
-        <v>21</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K22">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="D23" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="12">
         <v>55</v>
@@ -1364,26 +1318,22 @@
       <c r="J23" s="13">
         <v>1.04</v>
       </c>
-      <c r="K23" s="25">
-        <v>22</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="0"/>
+      <c r="K23">
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="16">
         <v>55</v>
@@ -1403,26 +1353,22 @@
       <c r="J24" s="17">
         <v>1.48</v>
       </c>
-      <c r="K24" s="24">
-        <v>29</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K24">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="C25" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" s="12">
         <v>55</v>
@@ -1442,26 +1388,22 @@
       <c r="J25" s="13">
         <v>1.55</v>
       </c>
-      <c r="K25" s="25">
-        <v>30</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="0"/>
+      <c r="K25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="12">
         <v>10</v>
@@ -1481,26 +1423,22 @@
       <c r="J26" s="13">
         <v>0.15</v>
       </c>
-      <c r="K26" s="25">
-        <v>4</v>
-      </c>
-      <c r="L26">
-        <f>G26/(3.14*0.45*0.45/4)</f>
-        <v>1.6985138004246285</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K26">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" s="12">
         <v>10</v>
@@ -1520,26 +1458,22 @@
       <c r="J27" s="13">
         <v>0.18</v>
       </c>
-      <c r="K27" s="25">
-        <v>6</v>
-      </c>
-      <c r="L27">
-        <f t="shared" ref="L27:L48" si="1">G27/(3.14*0.45*0.45/4)</f>
-        <v>1.25815837068491</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K27">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="C28" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>20</v>
-      </c>
       <c r="D28" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E28" s="16">
         <v>70</v>
@@ -1559,26 +1493,22 @@
       <c r="J28" s="17">
         <v>0.38</v>
       </c>
-      <c r="K28" s="24">
-        <v>9</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="1"/>
-        <v>1.5097900448218919</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K28">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>20</v>
-      </c>
       <c r="D29" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="12">
         <v>80</v>
@@ -1598,26 +1528,22 @@
       <c r="J29" s="13">
         <v>0.42</v>
       </c>
-      <c r="K29" s="25">
-        <v>10</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="1"/>
-        <v>1.4468821262876466</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K29">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" s="12">
         <v>50</v>
@@ -1637,26 +1563,22 @@
       <c r="J30" s="13">
         <v>0.48</v>
       </c>
-      <c r="K30" s="25">
-        <v>12</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="1"/>
-        <v>1.5097900448218919</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K30">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="16">
         <v>50</v>
@@ -1676,26 +1598,22 @@
       <c r="J31" s="17">
         <v>0.69</v>
       </c>
-      <c r="K31" s="24">
-        <v>15</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="1"/>
-        <v>1.6985138004246285</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K31">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" s="12">
         <v>80</v>
@@ -1715,26 +1633,22 @@
       <c r="J32" s="13">
         <v>0.75</v>
       </c>
-      <c r="K32" s="25">
-        <v>16</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="1"/>
-        <v>1.5097900448218919</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K32">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" s="12">
         <v>100</v>
@@ -1754,26 +1668,22 @@
       <c r="J33" s="13">
         <v>0.86</v>
       </c>
-      <c r="K33" s="25">
-        <v>18</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="1"/>
-        <v>2.0759613116301017</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K33">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" s="16">
         <v>80</v>
@@ -1793,26 +1703,22 @@
       <c r="J34" s="17">
         <v>0.94</v>
       </c>
-      <c r="K34" s="24">
+      <c r="K34">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L34">
-        <f t="shared" si="1"/>
-        <v>2.1388692301643468</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>20</v>
-      </c>
       <c r="D35" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E35" s="12">
         <v>70</v>
@@ -1832,26 +1738,22 @@
       <c r="J35" s="13">
         <v>0.98</v>
       </c>
-      <c r="K35" s="25">
-        <v>20</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="1"/>
-        <v>1.6985138004246285</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K35">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" s="16">
         <v>120</v>
@@ -1871,26 +1773,22 @@
       <c r="J36" s="17">
         <v>1.1200000000000001</v>
       </c>
-      <c r="K36" s="24">
-        <v>23</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="1"/>
-        <v>1.5097900448218919</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K36">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E37" s="12">
         <v>120</v>
@@ -1910,26 +1808,22 @@
       <c r="J37" s="13">
         <v>1.1399999999999999</v>
       </c>
-      <c r="K37" s="25">
-        <v>24</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="1"/>
-        <v>2.0130533930958561</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K37">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E38" s="16">
         <v>100</v>
@@ -1949,26 +1843,22 @@
       <c r="J38" s="17">
         <v>1.1399999999999999</v>
       </c>
-      <c r="K38" s="24">
-        <v>25</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="1"/>
-        <v>1.6985138004246285</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K38">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>20</v>
-      </c>
       <c r="D39" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E39" s="12">
         <v>100</v>
@@ -1988,26 +1878,22 @@
       <c r="J39" s="13">
         <v>1.2</v>
       </c>
-      <c r="K39" s="25">
-        <v>26</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="1"/>
-        <v>1.5097900448218919</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K39">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="C40" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>20</v>
-      </c>
       <c r="D40" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E40" s="16">
         <v>120</v>
@@ -2027,26 +1913,22 @@
       <c r="J40" s="17">
         <v>1.28</v>
       </c>
-      <c r="K40" s="24">
-        <v>27</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="1"/>
-        <v>1.4468821262876466</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K40">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="E41" s="12">
         <v>80</v>
@@ -2066,26 +1948,22 @@
       <c r="J41" s="13">
         <v>1.36</v>
       </c>
-      <c r="K41" s="25">
-        <v>28</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="1"/>
-        <v>1.5097900448218919</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K41">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" s="16">
         <v>70</v>
@@ -2105,26 +1983,22 @@
       <c r="J42" s="17">
         <v>1.68</v>
       </c>
-      <c r="K42" s="24">
-        <v>31</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="1"/>
-        <v>2.0130533930958561</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K42">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="E43" s="12">
         <v>100</v>
@@ -2144,26 +2018,22 @@
       <c r="J43" s="13">
         <v>1.74</v>
       </c>
-      <c r="K43" s="25">
-        <v>32</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="1"/>
-        <v>1.8243296374931193</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K43">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E44" s="16">
         <v>50</v>
@@ -2183,26 +2053,22 @@
       <c r="J44" s="17">
         <v>2.0499999999999998</v>
       </c>
-      <c r="K44" s="24">
-        <v>33</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="1"/>
-        <v>1.7614217189588741</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K44">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E45" s="12">
         <v>80</v>
@@ -2222,26 +2088,22 @@
       <c r="J45" s="13">
         <v>2.08</v>
       </c>
-      <c r="K45" s="25">
-        <v>34</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="1"/>
-        <v>2.0130533930958561</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K45">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E46" s="16">
         <v>100</v>
@@ -2261,26 +2123,22 @@
       <c r="J46" s="17">
         <v>2.12</v>
       </c>
-      <c r="K46" s="24">
-        <v>35</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="1"/>
-        <v>1.8243296374931193</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K46">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E47" s="12">
         <v>120</v>
@@ -2300,26 +2158,22 @@
       <c r="J47" s="13">
         <v>3.12</v>
       </c>
-      <c r="K47" s="25">
-        <v>36</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="1"/>
-        <v>2.0130533930958561</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K47">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="C48" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="15" t="s">
-        <v>32</v>
-      </c>
       <c r="D48" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E48" s="16">
         <v>400</v>
@@ -2339,21 +2193,16 @@
       <c r="J48" s="17">
         <v>4.45</v>
       </c>
-      <c r="K48" s="24">
-        <v>37</v>
-      </c>
-      <c r="L48">
-        <f>G48/(3.14*0.6*0.6/4)</f>
-        <v>0.88464260438782738</v>
+      <c r="K48">
+        <v>0.88</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:K48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:J48">
     <sortCondition ref="A12:A48"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="J9:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>